<commit_message>
run unit test cases in progress, change in data file and ddl file
</commit_message>
<xml_diff>
--- a/LearningManagementSystem/learners.xlsx
+++ b/LearningManagementSystem/learners.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="360" yWindow="150" windowWidth="2835" windowHeight="6735"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -30,26 +30,29 @@
     <t>Email</t>
   </si>
   <si>
-    <t>L&amp;D</t>
-  </si>
-  <si>
-    <t>Ted Mosby</t>
-  </si>
-  <si>
-    <t>R&amp;D</t>
-  </si>
-  <si>
-    <t>Sheldon Cooper</t>
-  </si>
-  <si>
-    <t>Put your email here</t>
+    <t>Akshay</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>akshay@gmail.com</t>
+  </si>
+  <si>
+    <t>Vinod</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>vinod@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,12 +64,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -93,17 +90,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -402,12 +398,12 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -417,7 +413,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -426,33 +422,37 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1">
-        <v>9876456723</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>7656787890</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1">
-        <v>9835672893</v>
-      </c>
-      <c r="D3" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="C3">
+        <v>7869352434</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>